<commit_message>
REST methods table updated
</commit_message>
<xml_diff>
--- a/REST_Instructions.xlsx
+++ b/REST_Instructions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dorin\Desktop\Greenhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>GET</t>
   </si>
@@ -81,6 +81,87 @@
   </si>
   <si>
     <t>Reset desired light value</t>
+  </si>
+  <si>
+    <t>temperature/mode</t>
+  </si>
+  <si>
+    <t>humidity/mode</t>
+  </si>
+  <si>
+    <t>light/mode</t>
+  </si>
+  <si>
+    <t>heater</t>
+  </si>
+  <si>
+    <t>lid</t>
+  </si>
+  <si>
+    <t>Get temperature control mode</t>
+  </si>
+  <si>
+    <t>Get humidity control mode</t>
+  </si>
+  <si>
+    <t>Get light control mode</t>
+  </si>
+  <si>
+    <t>Enable automatic light control</t>
+  </si>
+  <si>
+    <t>Enable automatic humidity control</t>
+  </si>
+  <si>
+    <t>Enable automatic temperature control</t>
+  </si>
+  <si>
+    <t>get lid state in degrees</t>
+  </si>
+  <si>
+    <t>lamp</t>
+  </si>
+  <si>
+    <t>get get lamp value in %</t>
+  </si>
+  <si>
+    <t>Enable manual heater control at a given value</t>
+  </si>
+  <si>
+    <t>Enable manual lig control at a given value</t>
+  </si>
+  <si>
+    <t>Enable manual lamp control at a given value</t>
+  </si>
+  <si>
+    <t>Toggle temperature control mode</t>
+  </si>
+  <si>
+    <t>Toggle humidity control mode</t>
+  </si>
+  <si>
+    <t>Toggle light control mode</t>
+  </si>
+  <si>
+    <t>Disable manual heater control</t>
+  </si>
+  <si>
+    <t>Disable manual lid control</t>
+  </si>
+  <si>
+    <t>Disable manual lamp control</t>
+  </si>
+  <si>
+    <t>Reset heater value</t>
+  </si>
+  <si>
+    <t>Reset lid value</t>
+  </si>
+  <si>
+    <t>Reset lamp value</t>
+  </si>
+  <si>
+    <t>Get heater value</t>
   </si>
 </sst>
 </file>
@@ -443,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,36 +569,138 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PUT methods removed from REST interface
</commit_message>
<xml_diff>
--- a/REST_Instructions.xlsx
+++ b/REST_Instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>GET</t>
   </si>
@@ -32,9 +32,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>PUT</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -53,36 +50,9 @@
     <t>Get humidity value in %</t>
   </si>
   <si>
-    <t>Disable automatic temperature control</t>
-  </si>
-  <si>
-    <t>Disable automatic humidity control</t>
-  </si>
-  <si>
-    <t>Disable automatic light level control</t>
-  </si>
-  <si>
     <t>Get light level raw value</t>
   </si>
   <si>
-    <t>Enable automatic temperature control at given value</t>
-  </si>
-  <si>
-    <t>Enable automatic humidity control at given value</t>
-  </si>
-  <si>
-    <t>Enable automatic light control at given value</t>
-  </si>
-  <si>
-    <t>Reset desired temperature value</t>
-  </si>
-  <si>
-    <t>Reset desired humidity value</t>
-  </si>
-  <si>
-    <t>Reset desired light value</t>
-  </si>
-  <si>
     <t>temperature/mode</t>
   </si>
   <si>
@@ -98,24 +68,6 @@
     <t>lid</t>
   </si>
   <si>
-    <t>Get temperature control mode</t>
-  </si>
-  <si>
-    <t>Get humidity control mode</t>
-  </si>
-  <si>
-    <t>Get light control mode</t>
-  </si>
-  <si>
-    <t>Enable automatic light control</t>
-  </si>
-  <si>
-    <t>Enable automatic humidity control</t>
-  </si>
-  <si>
-    <t>Enable automatic temperature control</t>
-  </si>
-  <si>
     <t>get lid state in degrees</t>
   </si>
   <si>
@@ -125,43 +77,52 @@
     <t>get get lamp value in %</t>
   </si>
   <si>
-    <t>Enable manual heater control at a given value</t>
-  </si>
-  <si>
-    <t>Enable manual lig control at a given value</t>
-  </si>
-  <si>
-    <t>Enable manual lamp control at a given value</t>
-  </si>
-  <si>
-    <t>Toggle temperature control mode</t>
-  </si>
-  <si>
-    <t>Toggle humidity control mode</t>
-  </si>
-  <si>
-    <t>Toggle light control mode</t>
-  </si>
-  <si>
-    <t>Disable manual heater control</t>
-  </si>
-  <si>
-    <t>Disable manual lid control</t>
-  </si>
-  <si>
-    <t>Disable manual lamp control</t>
-  </si>
-  <si>
-    <t>Reset heater value</t>
-  </si>
-  <si>
-    <t>Reset lid value</t>
-  </si>
-  <si>
-    <t>Reset lamp value</t>
-  </si>
-  <si>
     <t>Get heater value</t>
+  </si>
+  <si>
+    <t>Get temperature control mode [0 - manual, 1 - auto]</t>
+  </si>
+  <si>
+    <t>Get humidity control mode [0 - manual, 1 - auto]</t>
+  </si>
+  <si>
+    <t>Get light control mode [0 - manual, 1 - auto]</t>
+  </si>
+  <si>
+    <t>Automaticaly keep temperature at the given value</t>
+  </si>
+  <si>
+    <t>Automaticaly keep humidity at the given value</t>
+  </si>
+  <si>
+    <t>Automaticaly keep light at the given value</t>
+  </si>
+  <si>
+    <t>Automaticaly keep temperature at its current value</t>
+  </si>
+  <si>
+    <t>Automaticaly keep humidity at its current value</t>
+  </si>
+  <si>
+    <t>Automaticaly keep light at its current value</t>
+  </si>
+  <si>
+    <t>Manually set heater to the given value</t>
+  </si>
+  <si>
+    <t>Manually set lid to the given value</t>
+  </si>
+  <si>
+    <t>Manually set lamp to the given value</t>
+  </si>
+  <si>
+    <t>Disable automatic temperature control (disables heater)</t>
+  </si>
+  <si>
+    <t>Disable automatic humidity control (closes the lid)</t>
+  </si>
+  <si>
+    <t>Disable automatic light level control (turns off the lamp)</t>
   </si>
 </sst>
 </file>
@@ -524,19 +485,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="5" width="48.85546875" customWidth="1"/>
+    <col min="2" max="4" width="65.42578125" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,161 +508,131 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D10" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>